<commit_message>
Adding new notification test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Notifications.xlsx
+++ b/src/test/resources/xls/Notifications.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="103">
   <si>
     <t>TCID</t>
   </si>
@@ -176,9 +176,6 @@
     <t>OPQA-209</t>
   </si>
   <si>
-    <t>Y</t>
-  </si>
-  <si>
     <t>OPQA-877</t>
   </si>
   <si>
@@ -354,7 +351,25 @@
     <t>Notifications021</t>
   </si>
   <si>
-    <t>N</t>
+    <t>Verify that user is able to view top commenters information in home page</t>
+  </si>
+  <si>
+    <t>Notifications023</t>
+  </si>
+  <si>
+    <t>OPQA-211</t>
+  </si>
+  <si>
+    <t>Verify that user is able to view Most viewed documents in home page</t>
+  </si>
+  <si>
+    <t>Notifications024</t>
+  </si>
+  <si>
+    <t>OPQA-212</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
@@ -744,10 +759,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -778,7 +793,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>34</v>
@@ -787,15 +802,15 @@
         <v>30</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>38</v>
+        <v>102</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>35</v>
@@ -804,32 +819,32 @@
         <v>31</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>38</v>
+        <v>102</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>37</v>
@@ -838,299 +853,333 @@
         <v>32</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>40</v>
-      </c>
       <c r="D6" s="6" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>42</v>
-      </c>
       <c r="D7" s="6" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>36</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>49</v>
-      </c>
       <c r="D10" s="6" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>51</v>
-      </c>
       <c r="D11" s="6" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B12" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>53</v>
-      </c>
       <c r="D12" s="6" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B13" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>55</v>
-      </c>
       <c r="D13" s="6" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B16" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="D16" s="6" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="30">
       <c r="A17" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>63</v>
-      </c>
       <c r="D17" s="6" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B18" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="D18" s="6" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B19" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="D19" s="6" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B21" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="D21" s="6" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B22" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>70</v>
+      <c r="D23" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding watch list sanity test cases to Suite_G
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Notifications.xlsx
+++ b/src/test/resources/xls/Notifications.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="103">
   <si>
     <t>TCID</t>
   </si>
@@ -176,9 +176,6 @@
     <t>OPQA-209</t>
   </si>
   <si>
-    <t>Y</t>
-  </si>
-  <si>
     <t>OPQA-877</t>
   </si>
   <si>
@@ -354,7 +351,25 @@
     <t>Notifications021</t>
   </si>
   <si>
-    <t>N</t>
+    <t>Verify that user is able to view top commenters information in home page</t>
+  </si>
+  <si>
+    <t>Notifications023</t>
+  </si>
+  <si>
+    <t>OPQA-211</t>
+  </si>
+  <si>
+    <t>Verify that user is able to view Most viewed documents in home page</t>
+  </si>
+  <si>
+    <t>Notifications024</t>
+  </si>
+  <si>
+    <t>OPQA-212</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
@@ -744,10 +759,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -778,7 +793,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>34</v>
@@ -787,15 +802,15 @@
         <v>30</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>38</v>
+        <v>102</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>35</v>
@@ -804,32 +819,32 @@
         <v>31</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>38</v>
+        <v>102</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>37</v>
@@ -838,299 +853,333 @@
         <v>32</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>40</v>
-      </c>
       <c r="D6" s="6" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>42</v>
-      </c>
       <c r="D7" s="6" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>36</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>49</v>
-      </c>
       <c r="D10" s="6" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>51</v>
-      </c>
       <c r="D11" s="6" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B12" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>53</v>
-      </c>
       <c r="D12" s="6" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B13" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>55</v>
-      </c>
       <c r="D13" s="6" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B16" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="D16" s="6" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="30">
       <c r="A17" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>63</v>
-      </c>
       <c r="D17" s="6" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B18" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="D18" s="6" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B19" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="D19" s="6" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B21" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="D21" s="6" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B22" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>70</v>
+      <c r="D23" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding new test cases for Notifications
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Notifications.xlsx
+++ b/src/test/resources/xls/Notifications.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="109">
   <si>
     <t>TCID</t>
   </si>
@@ -370,6 +370,24 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>Verify that system is able to recommend six people for user</t>
+  </si>
+  <si>
+    <t>OPQA-1102</t>
+  </si>
+  <si>
+    <t>OPQA-1103</t>
+  </si>
+  <si>
+    <t>Verify that system is able to recommend three articles for user</t>
+  </si>
+  <si>
+    <t>Notifications022</t>
+  </si>
+  <si>
+    <t>Notifications025</t>
   </si>
 </sst>
 </file>
@@ -759,9 +777,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -1150,13 +1168,13 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="6" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>102</v>
@@ -1167,18 +1185,52 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B25" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D24" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="E24" s="6" t="s">
+      <c r="D25" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="E26" s="6" t="s">
         <v>72</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Enabling only Two test cases in Notifications
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Notifications.xlsx
+++ b/src/test/resources/xls/Notifications.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="110">
   <si>
     <t>TCID</t>
   </si>
@@ -388,6 +388,9 @@
   </si>
   <si>
     <t>Notifications025</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -780,7 +783,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -854,7 +857,7 @@
         <v>42</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>72</v>
@@ -871,7 +874,7 @@
         <v>32</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>72</v>
@@ -888,7 +891,7 @@
         <v>39</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>72</v>
@@ -905,7 +908,7 @@
         <v>41</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>72</v>
@@ -922,7 +925,7 @@
         <v>44</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>72</v>
@@ -939,7 +942,7 @@
         <v>45</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>72</v>
@@ -956,7 +959,7 @@
         <v>48</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>72</v>
@@ -973,7 +976,7 @@
         <v>50</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>72</v>
@@ -990,7 +993,7 @@
         <v>52</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>72</v>
@@ -1007,7 +1010,7 @@
         <v>54</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>72</v>
@@ -1024,7 +1027,7 @@
         <v>55</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>72</v>
@@ -1041,7 +1044,7 @@
         <v>57</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>72</v>
@@ -1058,7 +1061,7 @@
         <v>60</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>72</v>
@@ -1075,7 +1078,7 @@
         <v>62</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>72</v>
@@ -1092,7 +1095,7 @@
         <v>64</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>72</v>
@@ -1109,7 +1112,7 @@
         <v>66</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>72</v>
@@ -1126,7 +1129,7 @@
         <v>67</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>72</v>
@@ -1143,7 +1146,7 @@
         <v>71</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>72</v>
@@ -1160,7 +1163,7 @@
         <v>73</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>69</v>
@@ -1177,7 +1180,7 @@
         <v>103</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>72</v>
@@ -1194,7 +1197,7 @@
         <v>96</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>72</v>
@@ -1211,7 +1214,7 @@
         <v>99</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>72</v>
@@ -1228,7 +1231,7 @@
         <v>106</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>72</v>

</xml_diff>

<commit_message>
Running aall Notification test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Notifications.xlsx
+++ b/src/test/resources/xls/Notifications.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="109">
   <si>
     <t>TCID</t>
   </si>
@@ -388,9 +388,6 @@
   </si>
   <si>
     <t>Notifications025</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
 </sst>
 </file>
@@ -782,8 +779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -857,7 +854,7 @@
         <v>42</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>72</v>
@@ -874,7 +871,7 @@
         <v>32</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>72</v>
@@ -891,7 +888,7 @@
         <v>39</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>72</v>
@@ -908,7 +905,7 @@
         <v>41</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>72</v>
@@ -925,7 +922,7 @@
         <v>44</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>72</v>
@@ -942,7 +939,7 @@
         <v>45</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>72</v>
@@ -959,7 +956,7 @@
         <v>48</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>72</v>
@@ -976,7 +973,7 @@
         <v>50</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>72</v>
@@ -993,7 +990,7 @@
         <v>52</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>72</v>
@@ -1010,7 +1007,7 @@
         <v>54</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>72</v>
@@ -1027,7 +1024,7 @@
         <v>55</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>72</v>
@@ -1044,7 +1041,7 @@
         <v>57</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>72</v>
@@ -1061,7 +1058,7 @@
         <v>60</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>72</v>
@@ -1078,7 +1075,7 @@
         <v>62</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>72</v>
@@ -1095,7 +1092,7 @@
         <v>64</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>72</v>
@@ -1112,7 +1109,7 @@
         <v>66</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>72</v>
@@ -1129,7 +1126,7 @@
         <v>67</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>72</v>
@@ -1146,7 +1143,7 @@
         <v>71</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>72</v>
@@ -1163,7 +1160,7 @@
         <v>73</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>69</v>
@@ -1180,7 +1177,7 @@
         <v>103</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>72</v>
@@ -1197,7 +1194,7 @@
         <v>96</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>72</v>
@@ -1214,7 +1211,7 @@
         <v>99</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>72</v>
@@ -1231,7 +1228,7 @@
         <v>106</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>72</v>

</xml_diff>

<commit_message>
Running only 2 notification test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Notifications.xlsx
+++ b/src/test/resources/xls/Notifications.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="110">
   <si>
     <t>TCID</t>
   </si>
@@ -388,6 +388,9 @@
   </si>
   <si>
     <t>Notifications025</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -780,7 +783,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D26"/>
+      <selection activeCell="D4" sqref="D4:D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -854,7 +857,7 @@
         <v>42</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>72</v>
@@ -871,7 +874,7 @@
         <v>32</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>72</v>
@@ -888,7 +891,7 @@
         <v>39</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>72</v>
@@ -905,7 +908,7 @@
         <v>41</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>72</v>
@@ -922,7 +925,7 @@
         <v>44</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>72</v>
@@ -939,7 +942,7 @@
         <v>45</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>72</v>
@@ -956,7 +959,7 @@
         <v>48</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>72</v>
@@ -973,7 +976,7 @@
         <v>50</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>72</v>
@@ -990,7 +993,7 @@
         <v>52</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>72</v>
@@ -1007,7 +1010,7 @@
         <v>54</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>72</v>
@@ -1024,7 +1027,7 @@
         <v>55</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>72</v>
@@ -1041,7 +1044,7 @@
         <v>57</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>72</v>
@@ -1058,7 +1061,7 @@
         <v>60</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>72</v>
@@ -1075,7 +1078,7 @@
         <v>62</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>72</v>
@@ -1092,7 +1095,7 @@
         <v>64</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>72</v>
@@ -1109,7 +1112,7 @@
         <v>66</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>72</v>
@@ -1126,7 +1129,7 @@
         <v>67</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>72</v>
@@ -1143,7 +1146,7 @@
         <v>71</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>72</v>
@@ -1160,7 +1163,7 @@
         <v>73</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>69</v>
@@ -1177,7 +1180,7 @@
         <v>103</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>72</v>
@@ -1194,7 +1197,7 @@
         <v>96</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>72</v>
@@ -1211,7 +1214,7 @@
         <v>99</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>72</v>
@@ -1228,7 +1231,7 @@
         <v>106</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>72</v>

</xml_diff>

<commit_message>
Running all notification test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Notifications.xlsx
+++ b/src/test/resources/xls/Notifications.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="109">
   <si>
     <t>TCID</t>
   </si>
@@ -388,9 +388,6 @@
   </si>
   <si>
     <t>Notifications025</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
 </sst>
 </file>
@@ -783,7 +780,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:D26"/>
+      <selection activeCell="D2" sqref="D2:D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -857,7 +854,7 @@
         <v>42</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>72</v>
@@ -874,7 +871,7 @@
         <v>32</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>72</v>
@@ -891,7 +888,7 @@
         <v>39</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>72</v>
@@ -908,7 +905,7 @@
         <v>41</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>72</v>
@@ -925,7 +922,7 @@
         <v>44</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>72</v>
@@ -942,7 +939,7 @@
         <v>45</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>72</v>
@@ -959,7 +956,7 @@
         <v>48</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>72</v>
@@ -976,7 +973,7 @@
         <v>50</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>72</v>
@@ -993,7 +990,7 @@
         <v>52</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>72</v>
@@ -1010,7 +1007,7 @@
         <v>54</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>72</v>
@@ -1027,7 +1024,7 @@
         <v>55</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>72</v>
@@ -1044,7 +1041,7 @@
         <v>57</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>72</v>
@@ -1061,7 +1058,7 @@
         <v>60</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>72</v>
@@ -1078,7 +1075,7 @@
         <v>62</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>72</v>
@@ -1095,7 +1092,7 @@
         <v>64</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>72</v>
@@ -1112,7 +1109,7 @@
         <v>66</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>72</v>
@@ -1129,7 +1126,7 @@
         <v>67</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>72</v>
@@ -1146,7 +1143,7 @@
         <v>71</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>72</v>
@@ -1163,7 +1160,7 @@
         <v>73</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>69</v>
@@ -1180,7 +1177,7 @@
         <v>103</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>72</v>
@@ -1197,7 +1194,7 @@
         <v>96</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>72</v>
@@ -1214,7 +1211,7 @@
         <v>99</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>72</v>
@@ -1231,7 +1228,7 @@
         <v>106</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>72</v>

</xml_diff>

<commit_message>
running only one notification scenario
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Notifications.xlsx
+++ b/src/test/resources/xls/Notifications.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="110">
   <si>
     <t>TCID</t>
   </si>
@@ -388,6 +388,9 @@
   </si>
   <si>
     <t>Notifications025</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -780,7 +783,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D26"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -820,7 +823,7 @@
         <v>30</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>69</v>
@@ -837,7 +840,7 @@
         <v>31</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>72</v>
@@ -854,7 +857,7 @@
         <v>42</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>72</v>
@@ -871,7 +874,7 @@
         <v>32</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>72</v>
@@ -888,7 +891,7 @@
         <v>39</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>72</v>
@@ -905,7 +908,7 @@
         <v>41</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>72</v>
@@ -922,7 +925,7 @@
         <v>44</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>72</v>
@@ -939,7 +942,7 @@
         <v>45</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>72</v>
@@ -956,7 +959,7 @@
         <v>48</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>72</v>
@@ -973,7 +976,7 @@
         <v>50</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>72</v>
@@ -1007,7 +1010,7 @@
         <v>54</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>72</v>
@@ -1024,7 +1027,7 @@
         <v>55</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>72</v>
@@ -1041,7 +1044,7 @@
         <v>57</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>72</v>
@@ -1058,7 +1061,7 @@
         <v>60</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>72</v>
@@ -1075,7 +1078,7 @@
         <v>62</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>72</v>
@@ -1092,7 +1095,7 @@
         <v>64</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>72</v>
@@ -1109,7 +1112,7 @@
         <v>66</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>72</v>
@@ -1126,7 +1129,7 @@
         <v>67</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>72</v>
@@ -1143,7 +1146,7 @@
         <v>71</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>72</v>
@@ -1160,7 +1163,7 @@
         <v>73</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>69</v>
@@ -1177,7 +1180,7 @@
         <v>103</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>72</v>
@@ -1194,7 +1197,7 @@
         <v>96</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>72</v>
@@ -1211,7 +1214,7 @@
         <v>99</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>72</v>
@@ -1228,7 +1231,7 @@
         <v>106</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>72</v>

</xml_diff>

<commit_message>
Modified Test cases in to 1Pnotify created parallel test cases for notifications
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Notifications.xlsx
+++ b/src/test/resources/xls/Notifications.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="75">
   <si>
     <t>TCID</t>
   </si>
@@ -155,72 +155,18 @@
     <t>Verify that user receives a notification when he is followed by someone</t>
   </si>
   <si>
-    <t>Verify that user receives a notification when someone he is following comments on an article</t>
-  </si>
-  <si>
-    <t>Verify that user receives a notification if someone likes his comment</t>
-  </si>
-  <si>
     <t>Jira id</t>
   </si>
   <si>
     <t>OPQA-206</t>
   </si>
   <si>
-    <t>OPQA-207</t>
-  </si>
-  <si>
-    <t>OPQA-208</t>
-  </si>
-  <si>
-    <t>OPQA-209</t>
-  </si>
-  <si>
-    <t>OPQA-877</t>
-  </si>
-  <si>
-    <t>Verify that user receives a notification when someone he is following  publishes a post</t>
-  </si>
-  <si>
     <t>OPQA-213</t>
   </si>
   <si>
     <t>Verify that user is able to receive notification when my friend is following some other user.</t>
   </si>
   <si>
-    <t>Verify that user receives a notification when his follower comments on an article contained in his watchlist</t>
-  </si>
-  <si>
-    <t>OPQA-210</t>
-  </si>
-  <si>
-    <t>Verify that user receives a notification when someone comments on an article contained in his watchlist</t>
-  </si>
-  <si>
-    <t>Verify that user able to recevies a notification when other user commented on his post</t>
-  </si>
-  <si>
-    <t>OPQA-215</t>
-  </si>
-  <si>
-    <t>OPQA-216</t>
-  </si>
-  <si>
-    <t>Verify that user receives a notification when someone he is following user comments on a post</t>
-  </si>
-  <si>
-    <t>OPQA-217</t>
-  </si>
-  <si>
-    <t>Verify that user receives a notification when someone comments on an post contained in his watchlist</t>
-  </si>
-  <si>
-    <t>OPQA-218</t>
-  </si>
-  <si>
-    <t>Verify that user receives a notification if someone likes his comment on a post</t>
-  </si>
-  <si>
     <t>OPQA-1183</t>
   </si>
   <si>
@@ -231,12 +177,6 @@
   </si>
   <si>
     <t>OPQA-1184</t>
-  </si>
-  <si>
-    <t>Verify that user is receiving notification when someone liked his post(aggregated notification)</t>
-  </si>
-  <si>
-    <t>OPQA-1013</t>
   </si>
   <si>
     <t>OPQA-226</t>
@@ -264,108 +204,18 @@
     <t>Verify that Featured Post move down when new notification event occur</t>
   </si>
   <si>
-    <t>Verify that follower of the article is able to start conversation from home page when some one commented on the article he is following.</t>
-  </si>
-  <si>
-    <t>OPQA-1012</t>
-  </si>
-  <si>
     <t>PASS</t>
   </si>
   <si>
-    <t>OPQA-1011</t>
-  </si>
-  <si>
-    <t>Verify that follower of the post is able to start conversation from home page when some one commented on the post he is following.</t>
-  </si>
-  <si>
-    <t>SKIP</t>
-  </si>
-  <si>
-    <t>Verify that author of the post is able to start conversation from home page when some one commented on his post.</t>
-  </si>
-  <si>
-    <t>OPQA-1010</t>
-  </si>
-  <si>
-    <t>Notifications001</t>
-  </si>
-  <si>
-    <t>Notifications002</t>
-  </si>
-  <si>
-    <t>Notifications003</t>
-  </si>
-  <si>
-    <t>Notifications004</t>
-  </si>
-  <si>
-    <t>Notifications005</t>
-  </si>
-  <si>
-    <t>Notifications006</t>
-  </si>
-  <si>
-    <t>Notifications007</t>
-  </si>
-  <si>
-    <t>Notifications008</t>
-  </si>
-  <si>
-    <t>Notifications009</t>
-  </si>
-  <si>
-    <t>Notifications010</t>
-  </si>
-  <si>
-    <t>Notifications011</t>
-  </si>
-  <si>
-    <t>Notifications012</t>
-  </si>
-  <si>
-    <t>Notifications013</t>
-  </si>
-  <si>
-    <t>Notifications014</t>
-  </si>
-  <si>
-    <t>Notifications015</t>
-  </si>
-  <si>
-    <t>Notifications016</t>
-  </si>
-  <si>
-    <t>Notifications017</t>
-  </si>
-  <si>
-    <t>Notifications018</t>
-  </si>
-  <si>
-    <t>Notifications019</t>
-  </si>
-  <si>
-    <t>Notifications020</t>
-  </si>
-  <si>
-    <t>Notifications021</t>
-  </si>
-  <si>
     <t>Verify that user is able to view top commenters information in home page</t>
   </si>
   <si>
-    <t>Notifications023</t>
-  </si>
-  <si>
     <t>OPQA-211</t>
   </si>
   <si>
     <t>Verify that user is able to view Most viewed documents in home page</t>
   </si>
   <si>
-    <t>Notifications024</t>
-  </si>
-  <si>
     <t>OPQA-212</t>
   </si>
   <si>
@@ -384,10 +234,58 @@
     <t>Verify that system is able to recommend three articles for user</t>
   </si>
   <si>
-    <t>Notifications022</t>
-  </si>
-  <si>
-    <t>Notifications025</t>
+    <t>Notifications0001</t>
+  </si>
+  <si>
+    <t>Notifications0002</t>
+  </si>
+  <si>
+    <t>Notifications0003</t>
+  </si>
+  <si>
+    <t>Notifications0004</t>
+  </si>
+  <si>
+    <t>Notifications0005</t>
+  </si>
+  <si>
+    <t>Notifications0006</t>
+  </si>
+  <si>
+    <t>Notifications0007</t>
+  </si>
+  <si>
+    <t>Notifications0008</t>
+  </si>
+  <si>
+    <t>Notifications0009</t>
+  </si>
+  <si>
+    <t>Notifications0010</t>
+  </si>
+  <si>
+    <t>Notifications0011</t>
+  </si>
+  <si>
+    <t>Notifications0012</t>
+  </si>
+  <si>
+    <t>Notifications0013</t>
+  </si>
+  <si>
+    <t>Notifications0014</t>
+  </si>
+  <si>
+    <t>OPQA-877||OPQA-1013||OPQA-215</t>
+  </si>
+  <si>
+    <t>Verify that user receives a notification when someone he is following  publishes a post||Verify that user is receiving notification when someone liked his post(aggregated notification)||Verify that user able to recevies a notification when other user commented on his post</t>
+  </si>
+  <si>
+    <t>OPQA-208||OPQA-207||OPQA-209</t>
+  </si>
+  <si>
+    <t>Verify that user receives a notification when someone comments on an article contained in his watchlist||Verify that user receives a notification when someone he is following comments on an article||Verify that user receives a notification if someone likes his comment an article</t>
   </si>
 </sst>
 </file>
@@ -458,7 +356,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -478,6 +376,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -777,17 +679,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D26"/>
+      <selection activeCell="E14" sqref="E14:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="135.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="135.5703125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
@@ -797,9 +699,9 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="8" t="s">
@@ -811,427 +713,240 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="6" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="B3" s="6" t="s">
+      <c r="D5" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="E3" s="6" t="s">
+      <c r="C6" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30">
+      <c r="A8" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30">
+      <c r="A9" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>45</v>
-      </c>
       <c r="D9" s="6" t="s">
-        <v>102</v>
+        <v>52</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>72</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="6" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>48</v>
+        <v>39</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>102</v>
+        <v>52</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="30">
       <c r="A11" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>50</v>
+        <v>66</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>102</v>
+        <v>52</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>72</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="6" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>52</v>
+        <v>43</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>102</v>
+        <v>52</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>72</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="6" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="B13" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>54</v>
-      </c>
       <c r="D13" s="6" t="s">
-        <v>102</v>
+        <v>52</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>72</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="6" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="B14" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="D14" s="6" t="s">
-        <v>102</v>
+        <v>52</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>72</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="6" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>57</v>
+        <v>45</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>46</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>102</v>
+        <v>52</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="30">
-      <c r="A17" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>72</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added test cases in to 1PNOTIFY
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Notifications.xlsx
+++ b/src/test/resources/xls/Notifications.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="4230" yWindow="3960" windowWidth="14400" windowHeight="10125"/>
+    <workbookView xWindow="4236" yWindow="3960" windowWidth="14400" windowHeight="10128"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="82">
   <si>
     <t>TCID</t>
   </si>
@@ -286,6 +286,27 @@
   </si>
   <si>
     <t>Verify that user receives a notification when someone comments on an article contained in his watchlist||Verify that user receives a notification when someone he is following comments on an article||Verify that user receives a notification if someone likes his comment an article</t>
+  </si>
+  <si>
+    <t>Notifications0015</t>
+  </si>
+  <si>
+    <t>Notifications0016</t>
+  </si>
+  <si>
+    <t>OPQA-1603</t>
+  </si>
+  <si>
+    <t>Verify that user is able to navigate profile page by clicking author name in Recommended people to follow section on home page.</t>
+  </si>
+  <si>
+    <t>OPQA-1604</t>
+  </si>
+  <si>
+    <t>Verify that user is able to follow people from Recommended people to follow section on home page.</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -679,19 +700,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14:E15"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="135.5703125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="135.5546875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.33203125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -722,7 +743,7 @@
         <v>48</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>47</v>
@@ -739,7 +760,7 @@
         <v>50</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>47</v>
@@ -756,7 +777,7 @@
         <v>30</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>47</v>
@@ -773,7 +794,7 @@
         <v>34</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>47</v>
@@ -790,7 +811,7 @@
         <v>36</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>47</v>
@@ -807,13 +828,13 @@
         <v>37</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="30">
+    <row r="8" spans="1:5" ht="28.8">
       <c r="A8" s="9" t="s">
         <v>63</v>
       </c>
@@ -824,13 +845,13 @@
         <v>74</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="30">
+    <row r="9" spans="1:5" ht="28.8">
       <c r="A9" s="9" t="s">
         <v>64</v>
       </c>
@@ -841,7 +862,7 @@
         <v>72</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>47</v>
@@ -858,13 +879,13 @@
         <v>40</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="30">
+    <row r="11" spans="1:5" ht="28.8">
       <c r="A11" s="6" t="s">
         <v>66</v>
       </c>
@@ -875,7 +896,7 @@
         <v>42</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>47</v>
@@ -892,7 +913,7 @@
         <v>44</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>47</v>
@@ -909,7 +930,7 @@
         <v>53</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>47</v>
@@ -926,7 +947,7 @@
         <v>56</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>47</v>
@@ -943,9 +964,43 @@
         <v>46</v>
       </c>
       <c r="D15" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D16" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E16" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17" s="6" t="s">
         <v>47</v>
       </c>
     </row>
@@ -963,12 +1018,12 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="12" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="52.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="83.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.140625" style="4" collapsed="1"/>
+    <col min="2" max="2" width="52.5546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="83.88671875" style="4" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.109375" style="4" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="35.25" customHeight="1">
@@ -1037,7 +1092,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="60">
+    <row r="7" spans="1:3" ht="57.6">
       <c r="A7" s="3" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
Enabling notification test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Notifications.xlsx
+++ b/src/test/resources/xls/Notifications.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="4236" yWindow="3960" windowWidth="14400" windowHeight="10128"/>
+    <workbookView xWindow="4230" yWindow="3960" windowWidth="14400" windowHeight="10125"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="81">
   <si>
     <t>TCID</t>
   </si>
@@ -304,9 +304,6 @@
   </si>
   <si>
     <t>Verify that user is able to follow people from Recommended people to follow section on home page.</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
 </sst>
 </file>
@@ -702,17 +699,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="135.5546875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="135.5703125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -743,7 +740,7 @@
         <v>48</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>47</v>
@@ -760,7 +757,7 @@
         <v>50</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>47</v>
@@ -777,7 +774,7 @@
         <v>30</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>47</v>
@@ -794,7 +791,7 @@
         <v>34</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>47</v>
@@ -811,7 +808,7 @@
         <v>36</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>47</v>
@@ -828,13 +825,13 @@
         <v>37</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="28.8">
+    <row r="8" spans="1:5" ht="30">
       <c r="A8" s="9" t="s">
         <v>63</v>
       </c>
@@ -845,13 +842,13 @@
         <v>74</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="28.8">
+    <row r="9" spans="1:5" ht="30">
       <c r="A9" s="9" t="s">
         <v>64</v>
       </c>
@@ -862,7 +859,7 @@
         <v>72</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>47</v>
@@ -879,13 +876,13 @@
         <v>40</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="28.8">
+    <row r="11" spans="1:5" ht="30">
       <c r="A11" s="6" t="s">
         <v>66</v>
       </c>
@@ -896,7 +893,7 @@
         <v>42</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>47</v>
@@ -913,7 +910,7 @@
         <v>44</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>47</v>
@@ -930,7 +927,7 @@
         <v>53</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>47</v>
@@ -947,7 +944,7 @@
         <v>56</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>47</v>
@@ -964,7 +961,7 @@
         <v>46</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>47</v>
@@ -1018,12 +1015,12 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="52.5546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="83.88671875" style="4" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.109375" style="4" collapsed="1"/>
+    <col min="2" max="2" width="52.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="83.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="4" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="35.25" customHeight="1">
@@ -1092,7 +1089,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="57.6">
+    <row r="7" spans="1:3" ht="60">
       <c r="A7" s="3" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
Added test cases in to Notification module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Notifications.xlsx
+++ b/src/test/resources/xls/Notifications.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="4230" yWindow="3960" windowWidth="14400" windowHeight="10125"/>
+    <workbookView xWindow="4236" yWindow="3960" windowWidth="14400" windowHeight="10128"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="90">
   <si>
     <t>TCID</t>
   </si>
@@ -304,6 +304,33 @@
   </si>
   <si>
     <t>Verify that user is able to follow people from Recommended people to follow section on home page.</t>
+  </si>
+  <si>
+    <t>Notifications0017</t>
+  </si>
+  <si>
+    <t>OPQA-1601</t>
+  </si>
+  <si>
+    <t>Verify that user is able to navigate record view page by clicking article title from Recommended articles section on Home page</t>
+  </si>
+  <si>
+    <t>Notifications0018</t>
+  </si>
+  <si>
+    <t>OPQA-1602</t>
+  </si>
+  <si>
+    <t>Verify that user is able to watch article from Recommended articles section on Home page.</t>
+  </si>
+  <si>
+    <t>Notifications0019</t>
+  </si>
+  <si>
+    <t>OPQA-1600</t>
+  </si>
+  <si>
+    <t>Verify that user ia able to publish post by clicking "Publish a post of your own" link Feature post section on Home page.</t>
   </si>
 </sst>
 </file>
@@ -697,19 +724,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D15"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="135.5703125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="135.5546875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.33203125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -831,7 +858,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="30">
+    <row r="8" spans="1:5" ht="28.8">
       <c r="A8" s="9" t="s">
         <v>63</v>
       </c>
@@ -848,7 +875,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="30">
+    <row r="9" spans="1:5" ht="28.8">
       <c r="A9" s="9" t="s">
         <v>64</v>
       </c>
@@ -882,7 +909,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="30">
+    <row r="11" spans="1:5" ht="28.8">
       <c r="A11" s="6" t="s">
         <v>66</v>
       </c>
@@ -998,6 +1025,57 @@
         <v>52</v>
       </c>
       <c r="E17" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" s="6" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1015,12 +1093,12 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="12" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="52.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="83.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.140625" style="4" collapsed="1"/>
+    <col min="2" max="2" width="52.5546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="83.88671875" style="4" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.109375" style="4" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="35.25" customHeight="1">
@@ -1089,7 +1167,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="60">
+    <row r="7" spans="1:3" ht="57.6">
       <c r="A7" s="3" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
Added test cases in to notifications
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Notifications.xlsx
+++ b/src/test/resources/xls/Notifications.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="4236" yWindow="3960" windowWidth="14400" windowHeight="10128"/>
+    <workbookView xWindow="4230" yWindow="3960" windowWidth="14400" windowHeight="10125"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="94">
   <si>
     <t>TCID</t>
   </si>
@@ -331,6 +331,18 @@
   </si>
   <si>
     <t>Verify that user ia able to publish post by clicking "Publish a post of your own" link Feature post section on Home page.</t>
+  </si>
+  <si>
+    <t>OPQA-216||OPQA-217||OPQA-218</t>
+  </si>
+  <si>
+    <t>Verify that user receives a notification when someone he is following user comments on a post|| Verify that user receives a notification when someone comments on an post contained in his watchlist||Verify that user receives a notification if someone likes his comment on a post</t>
+  </si>
+  <si>
+    <t>Notifications0020</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -724,26 +736,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="135.5546875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.85546875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="135.5703125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="10" t="s">
         <v>31</v>
       </c>
       <c r="C1" s="10" t="s">
@@ -760,7 +772,7 @@
       <c r="A2" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>49</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -777,7 +789,7 @@
       <c r="A3" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="7" t="s">
         <v>51</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -794,7 +806,7 @@
       <c r="A4" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="7" t="s">
         <v>32</v>
       </c>
       <c r="C4" s="7" t="s">
@@ -811,7 +823,7 @@
       <c r="A5" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="7" t="s">
         <v>33</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -828,7 +840,7 @@
       <c r="A6" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="7" t="s">
         <v>35</v>
       </c>
       <c r="C6" s="7" t="s">
@@ -845,7 +857,7 @@
       <c r="A7" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="7" t="s">
         <v>38</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -858,7 +870,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="28.8">
+    <row r="8" spans="1:5" ht="30">
       <c r="A8" s="9" t="s">
         <v>63</v>
       </c>
@@ -875,7 +887,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="28.8">
+    <row r="9" spans="1:5" ht="30">
       <c r="A9" s="9" t="s">
         <v>64</v>
       </c>
@@ -896,7 +908,7 @@
       <c r="A10" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="7" t="s">
         <v>39</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -909,11 +921,11 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="28.8">
+    <row r="11" spans="1:5" ht="30">
       <c r="A11" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="3" t="s">
         <v>41</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -930,7 +942,7 @@
       <c r="A12" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="7" t="s">
         <v>43</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -947,7 +959,7 @@
       <c r="A13" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="7" t="s">
         <v>54</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -964,7 +976,7 @@
       <c r="A14" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="7" t="s">
         <v>55</v>
       </c>
       <c r="C14" s="3" t="s">
@@ -981,14 +993,14 @@
       <c r="A15" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="7" t="s">
         <v>46</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>52</v>
+        <v>93</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>47</v>
@@ -998,10 +1010,10 @@
       <c r="A16" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="7" t="s">
         <v>78</v>
       </c>
       <c r="D16" s="6" t="s">
@@ -1015,10 +1027,10 @@
       <c r="A17" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="7" t="s">
         <v>80</v>
       </c>
       <c r="D17" s="6" t="s">
@@ -1032,10 +1044,10 @@
       <c r="A18" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="7" t="s">
         <v>83</v>
       </c>
       <c r="D18" s="6" t="s">
@@ -1049,10 +1061,10 @@
       <c r="A19" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="7" t="s">
         <v>86</v>
       </c>
       <c r="D19" s="6" t="s">
@@ -1066,16 +1078,33 @@
       <c r="A20" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="7" t="s">
         <v>89</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>52</v>
       </c>
       <c r="E20" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="30">
+      <c r="A21" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E21" s="6" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1093,12 +1122,12 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="52.5546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="83.88671875" style="4" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.109375" style="4" collapsed="1"/>
+    <col min="2" max="2" width="52.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="83.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="4" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="35.25" customHeight="1">
@@ -1167,7 +1196,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="57.6">
+    <row r="7" spans="1:3" ht="60">
       <c r="A7" s="3" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
Modified test scripts into notifications
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Notifications.xlsx
+++ b/src/test/resources/xls/Notifications.xlsx
@@ -339,10 +339,10 @@
     <t>N</t>
   </si>
   <si>
-    <t>Verify that user receives a notification when someone he is following  publishes a post||Verify that user is receiving notification when someone liked his post(aggregated notification)||Verify that user able to recevies a notification when other user commented on his post||Verify that all users receive notification when other user published a comment on post and validate notification.||Verify that all users receive notification when other user published a post and validate notification.</t>
-  </si>
-  <si>
-    <t>OPQA-877||OPQA-1013||OPQA-215||OPQA-1397||OPQA-1395</t>
+    <t>OPQA-877||OPQA-1013||OPQA-215||OPQA-1395</t>
+  </si>
+  <si>
+    <t>Verify that user receives a notification when someone he is following  publishes a post||Verify that user is receiving notification when someone liked his post(aggregated notification)||Verify that user able to recevies a notification when other user commented on his post||Verify that all users receive notification when other user published a post and validate notification.</t>
   </si>
 </sst>
 </file>
@@ -739,7 +739,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -887,15 +887,15 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="60">
+    <row r="9" spans="1:5" ht="45">
       <c r="A9" s="9" t="s">
         <v>64</v>
       </c>
       <c r="B9" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>93</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>92</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>52</v>

</xml_diff>

<commit_message>
Fixed scripts in Notification Module.
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Notifications.xlsx
+++ b/src/test/resources/xls/Notifications.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="106">
   <si>
     <t>TCID</t>
   </si>
@@ -370,6 +370,15 @@
   </si>
   <si>
     <t>Verify that user receives a notification when someone he is following publishes a post||Verify that user is receiving notification when someone liked his post(aggregated notification)||Verify that user able to recevies a notification when other user commented on his post||Verify that all users receive notification when other user published a post and validate notification.||Verify that author of the post is able to start conversation from home page when some one commented on his post.</t>
+  </si>
+  <si>
+    <t>Notifications0021</t>
+  </si>
+  <si>
+    <t>OPQA-1433||OPQA-1432</t>
+  </si>
+  <si>
+    <t>Verify that user receives a notification when someone he is following comments on a patent||Verify that user receives a notification when someone comments on a patent contained in his watchlist</t>
   </si>
 </sst>
 </file>
@@ -763,10 +772,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C3" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1135,15 +1144,15 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" ht="28.8">
       <c r="A22" s="6" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>51</v>
@@ -1154,13 +1163,13 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="6" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>51</v>
@@ -1171,18 +1180,35 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B25" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C25" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="D24" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E24" s="6" t="s">
+      <c r="D25" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E25" s="6" t="s">
         <v>46</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changed Notification excel file.
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Notifications.xlsx
+++ b/src/test/resources/xls/Notifications.xlsx
@@ -774,8 +774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1121,7 +1121,7 @@
         <v>85</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>51</v>
+        <v>87</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>46</v>

</xml_diff>

<commit_message>
Modified Test scritps in IAM and ENWIAM Module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Notifications.xlsx
+++ b/src/test/resources/xls/Notifications.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="4230" yWindow="3960" windowWidth="14400" windowHeight="10125"/>
+    <workbookView xWindow="4236" yWindow="3960" windowWidth="14400" windowHeight="10128"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -248,13 +248,13 @@
     <t>Notifications0021</t>
   </si>
   <si>
-    <t>OPQA-1433||OPQA-1432</t>
-  </si>
-  <si>
-    <t>Verify that user receives a notification when someone he is following comments on a patent||Verify that user receives a notification when someone comments on a patent contained in his watchlist</t>
-  </si>
-  <si>
     <t>OPQA-231||OPQA-1100</t>
+  </si>
+  <si>
+    <t>OPQA-1433||OPQA-1432||OPQA-3951</t>
+  </si>
+  <si>
+    <t>Verify that user receives a notification when someone he is following comments on a patent||Verify that user receives a notification when someone comments on a patent contained in his watchlist||Verify that user receives a notification if someone likes his comment an patent</t>
   </si>
 </sst>
 </file>
@@ -635,17 +635,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="C9" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="135.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.88671875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="135.5546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.33203125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -767,7 +767,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="30">
+    <row r="8" spans="1:5" ht="28.8">
       <c r="A8" s="6" t="s">
         <v>35</v>
       </c>
@@ -784,7 +784,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="60">
+    <row r="9" spans="1:5" ht="57.6">
       <c r="A9" s="6" t="s">
         <v>36</v>
       </c>
@@ -818,12 +818,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="30">
+    <row r="11" spans="1:5" ht="28.8">
       <c r="A11" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>61</v>
@@ -988,7 +988,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="45">
+    <row r="21" spans="1:5" ht="43.2">
       <c r="A21" s="3" t="s">
         <v>59</v>
       </c>
@@ -1005,15 +1005,15 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="30">
+    <row r="22" spans="1:5" ht="28.8">
       <c r="A22" s="3" t="s">
         <v>76</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
Added New Scripts in Notification Module.
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Notifications.xlsx
+++ b/src/test/resources/xls/Notifications.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="86">
   <si>
     <t>TCID</t>
   </si>
@@ -255,6 +255,24 @@
   </si>
   <si>
     <t>Verify that user receives a notification when someone he is following comments on a patent||Verify that user receives a notification when someone comments on a patent contained in his watchlist||Verify that user receives a notification if someone likes his comment an patent</t>
+  </si>
+  <si>
+    <t>Notifications0025</t>
+  </si>
+  <si>
+    <t>OPQA-4493</t>
+  </si>
+  <si>
+    <t>Verify that user navigate to record view page of the article while clicking article in trending section from Newsfeed page.</t>
+  </si>
+  <si>
+    <t>Notifications0026</t>
+  </si>
+  <si>
+    <t>Verify that user navigate to record view page of the post while clicking post in trending section from Newsfeed page.</t>
+  </si>
+  <si>
+    <t>OPQA-4499</t>
   </si>
 </sst>
 </file>
@@ -633,10 +651,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C9" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1073,6 +1091,40 @@
         <v>19</v>
       </c>
     </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>